<commit_message>
Lookup - Vlookup, Hlookup, Index
</commit_message>
<xml_diff>
--- a/Excel/Data files/Lecture_3_logical.xlsx
+++ b/Excel/Data files/Lecture_3_logical.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ds_30\Excel\Data files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E1BE9F-D3CF-4EE1-A66E-DD335D9CA8B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD17A89A-2846-499D-885D-C6B0C52BFD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="862" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="862" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AND OR" sheetId="2" r:id="rId1"/>
@@ -564,6 +564,9 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -617,9 +620,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1533,10 +1533,10 @@
   <sheetData>
     <row r="1" spans="1:28" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="56"/>
+      <c r="C1" s="38"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -1544,25 +1544,25 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="56" t="s">
+      <c r="K1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
       <c r="Q1" s="15"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="56"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
       <c r="AB1" s="15"/>
     </row>
     <row r="2" spans="1:28" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -1580,13 +1580,13 @@
     </row>
     <row r="4" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="14"/>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="41"/>
       <c r="H4" s="14"/>
       <c r="I4" s="10"/>
       <c r="J4" s="18"/>
@@ -1615,11 +1615,11 @@
     </row>
     <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="43"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="44"/>
       <c r="H5" s="3"/>
       <c r="I5" s="11"/>
       <c r="J5" s="19"/>
@@ -1650,11 +1650,11 @@
       </c>
     </row>
     <row r="6" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="41"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="43"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="44"/>
       <c r="L6" s="24" t="s">
         <v>18</v>
       </c>
@@ -1681,11 +1681,11 @@
       </c>
     </row>
     <row r="7" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="41"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="43"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="44"/>
       <c r="L7" s="24" t="s">
         <v>19</v>
       </c>
@@ -1712,11 +1712,11 @@
       </c>
     </row>
     <row r="8" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="41"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="43"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="44"/>
       <c r="L8" s="24" t="s">
         <v>20</v>
       </c>
@@ -1743,11 +1743,11 @@
       </c>
     </row>
     <row r="9" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="41"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="43"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="44"/>
       <c r="L9" s="24" t="s">
         <v>21</v>
       </c>
@@ -1774,19 +1774,19 @@
       </c>
     </row>
     <row r="10" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="41"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="43"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="44"/>
     </row>
     <row r="11" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="46"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="47"/>
     </row>
     <row r="12" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B12" s="4"/>
@@ -1797,78 +1797,78 @@
     </row>
     <row r="14" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="47" t="s">
+      <c r="C14" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="50"/>
     </row>
     <row r="15" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="52"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="53"/>
     </row>
     <row r="16" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="52"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="53"/>
     </row>
     <row r="17" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="50"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="52"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="53"/>
     </row>
     <row r="18" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="50"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="52"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="53"/>
     </row>
     <row r="19" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="50"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="52"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="53"/>
     </row>
     <row r="20" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="50"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="52"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="53"/>
     </row>
     <row r="21" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="53"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="55"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
     <mergeCell ref="C4:G11"/>
     <mergeCell ref="C14:G21"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1879,8 +1879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="72" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="72" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1915,23 +1915,23 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="56" t="s">
+      <c r="K1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="56"/>
+      <c r="L1" s="38"/>
       <c r="M1" s="15"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
       <c r="Z1" s="15"/>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -2175,13 +2175,13 @@
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="47" t="s">
+      <c r="C14" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="50"/>
       <c r="L14" s="29" t="s">
         <v>17</v>
       </c>
@@ -2205,11 +2205,11 @@
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="52"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="53"/>
       <c r="L15" s="29" t="s">
         <v>18</v>
       </c>
@@ -2233,11 +2233,11 @@
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="52"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="53"/>
       <c r="L16" s="29" t="s">
         <v>19</v>
       </c>
@@ -2260,11 +2260,11 @@
       </c>
     </row>
     <row r="17" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="50"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="52"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="53"/>
       <c r="L17" s="29" t="s">
         <v>20</v>
       </c>
@@ -2287,11 +2287,11 @@
       </c>
     </row>
     <row r="18" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="50"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="52"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="53"/>
       <c r="L18" s="29" t="s">
         <v>21</v>
       </c>
@@ -2314,25 +2314,25 @@
       </c>
     </row>
     <row r="19" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="50"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="52"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="53"/>
     </row>
     <row r="20" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="50"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="52"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="53"/>
     </row>
     <row r="21" spans="3:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="53"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="55"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2391,24 +2391,24 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="56" t="s">
+      <c r="K1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
       <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -2637,13 +2637,13 @@
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="47" t="s">
+      <c r="C14" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="50"/>
       <c r="L14" s="28" t="s">
         <v>29</v>
       </c>
@@ -2659,11 +2659,11 @@
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="52"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="53"/>
       <c r="L15" s="22" t="s">
         <v>30</v>
       </c>
@@ -2679,11 +2679,11 @@
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="52"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="53"/>
       <c r="L16" s="22" t="s">
         <v>31</v>
       </c>
@@ -2698,11 +2698,11 @@
       <c r="O16" s="24"/>
     </row>
     <row r="17" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="50"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="52"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="53"/>
       <c r="L17" s="22" t="s">
         <v>32</v>
       </c>
@@ -2717,36 +2717,36 @@
       <c r="O17" s="24"/>
     </row>
     <row r="18" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="50"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="52"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="53"/>
     </row>
     <row r="19" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C19" s="50"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="52"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="53"/>
       <c r="L19" s="26" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="20" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="50"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="52"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="53"/>
       <c r="L20" s="30"/>
     </row>
     <row r="21" spans="3:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="53"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="55"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="56"/>
       <c r="L21" s="31" t="s">
         <v>39</v>
       </c>
@@ -2782,7 +2782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="66" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="66" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
@@ -2815,23 +2815,23 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="56" t="s">
+      <c r="K1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
       <c r="O1" s="15"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
       <c r="Z1" s="15"/>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -3073,13 +3073,13 @@
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="47" t="s">
+      <c r="C14" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="50"/>
       <c r="L14" s="21" t="b">
         <v>0</v>
       </c>
@@ -3098,54 +3098,54 @@
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="52"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="53"/>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="52"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="53"/>
     </row>
     <row r="17" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="50"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="52"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="53"/>
     </row>
     <row r="18" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="50"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="52"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="53"/>
     </row>
     <row r="19" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="50"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="52"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="53"/>
     </row>
     <row r="20" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="50"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="52"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="53"/>
     </row>
     <row r="21" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="53"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="55"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
Charts - Bar, Line, Scatter,
</commit_message>
<xml_diff>
--- a/Excel/Data files/Lecture_3_logical.xlsx
+++ b/Excel/Data files/Lecture_3_logical.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ds_30\Excel\Data files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD17A89A-2846-499D-885D-C6B0C52BFD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFB5947-D645-48B6-9884-98BAF21F2958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="862" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -564,62 +564,62 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1533,10 +1533,10 @@
   <sheetData>
     <row r="1" spans="1:28" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="38"/>
+      <c r="C1" s="56"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -1544,25 +1544,25 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="38" t="s">
+      <c r="K1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
       <c r="Q1" s="15"/>
-      <c r="R1" s="38"/>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="38"/>
-      <c r="AA1" s="38"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+      <c r="AA1" s="56"/>
       <c r="AB1" s="15"/>
     </row>
     <row r="2" spans="1:28" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -1580,13 +1580,13 @@
     </row>
     <row r="4" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="14"/>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="41"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="40"/>
       <c r="H4" s="14"/>
       <c r="I4" s="10"/>
       <c r="J4" s="18"/>
@@ -1615,11 +1615,11 @@
     </row>
     <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="44"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="43"/>
       <c r="H5" s="3"/>
       <c r="I5" s="11"/>
       <c r="J5" s="19"/>
@@ -1650,11 +1650,11 @@
       </c>
     </row>
     <row r="6" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="42"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="44"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="43"/>
       <c r="L6" s="24" t="s">
         <v>18</v>
       </c>
@@ -1681,11 +1681,11 @@
       </c>
     </row>
     <row r="7" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="42"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="44"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="43"/>
       <c r="L7" s="24" t="s">
         <v>19</v>
       </c>
@@ -1712,11 +1712,11 @@
       </c>
     </row>
     <row r="8" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="42"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="44"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="43"/>
       <c r="L8" s="24" t="s">
         <v>20</v>
       </c>
@@ -1743,11 +1743,11 @@
       </c>
     </row>
     <row r="9" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="42"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="44"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="43"/>
       <c r="L9" s="24" t="s">
         <v>21</v>
       </c>
@@ -1774,19 +1774,19 @@
       </c>
     </row>
     <row r="10" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="42"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="44"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="43"/>
     </row>
     <row r="11" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="47"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="46"/>
     </row>
     <row r="12" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B12" s="4"/>
@@ -1797,78 +1797,78 @@
     </row>
     <row r="14" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="50"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="49"/>
     </row>
     <row r="15" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="53"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="52"/>
     </row>
     <row r="16" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="53"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="52"/>
     </row>
     <row r="17" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="51"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="53"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="52"/>
     </row>
     <row r="18" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="51"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="53"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="52"/>
     </row>
     <row r="19" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="51"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="53"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="52"/>
     </row>
     <row r="20" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="51"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="53"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="52"/>
     </row>
     <row r="21" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="54"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="56"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
     <mergeCell ref="C4:G11"/>
     <mergeCell ref="C14:G21"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1879,8 +1879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="72" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="109" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1915,23 +1915,23 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="38" t="s">
+      <c r="K1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="38"/>
+      <c r="L1" s="56"/>
       <c r="M1" s="15"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
       <c r="Z1" s="15"/>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -2038,7 +2038,7 @@
         <v>B</v>
       </c>
       <c r="Q6" s="22" t="str">
-        <f t="shared" ref="Q6:Q9" si="1">IF(N6&gt;=85,"A",IF(N6&lt;60,"C","B"))</f>
+        <f>IF(N6&gt;=85,"A",IF(N6&lt;60,"C","B"))</f>
         <v>C</v>
       </c>
       <c r="R6" s="22"/>
@@ -2066,7 +2066,7 @@
         <v>A</v>
       </c>
       <c r="Q7" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="Q6:Q9" si="1">IF(N7&gt;=85,"A",IF(N7&lt;60,"C","B"))</f>
         <v>B</v>
       </c>
       <c r="R7" s="22"/>
@@ -2175,13 +2175,13 @@
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="50"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="49"/>
       <c r="L14" s="29" t="s">
         <v>17</v>
       </c>
@@ -2205,11 +2205,11 @@
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="53"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="52"/>
       <c r="L15" s="29" t="s">
         <v>18</v>
       </c>
@@ -2233,11 +2233,11 @@
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="53"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="52"/>
       <c r="L16" s="29" t="s">
         <v>19</v>
       </c>
@@ -2260,11 +2260,11 @@
       </c>
     </row>
     <row r="17" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="51"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="53"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="52"/>
       <c r="L17" s="29" t="s">
         <v>20</v>
       </c>
@@ -2287,11 +2287,11 @@
       </c>
     </row>
     <row r="18" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="51"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="53"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="52"/>
       <c r="L18" s="29" t="s">
         <v>21</v>
       </c>
@@ -2314,25 +2314,25 @@
       </c>
     </row>
     <row r="19" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="51"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="53"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="52"/>
     </row>
     <row r="20" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="51"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="53"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="52"/>
     </row>
     <row r="21" spans="3:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="54"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="56"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2391,24 +2391,24 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="38" t="s">
+      <c r="K1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="38"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
       <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -2637,13 +2637,13 @@
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="50"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="49"/>
       <c r="L14" s="28" t="s">
         <v>29</v>
       </c>
@@ -2659,11 +2659,11 @@
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="53"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="52"/>
       <c r="L15" s="22" t="s">
         <v>30</v>
       </c>
@@ -2679,11 +2679,11 @@
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="53"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="52"/>
       <c r="L16" s="22" t="s">
         <v>31</v>
       </c>
@@ -2698,11 +2698,11 @@
       <c r="O16" s="24"/>
     </row>
     <row r="17" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="51"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="53"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="52"/>
       <c r="L17" s="22" t="s">
         <v>32</v>
       </c>
@@ -2717,36 +2717,36 @@
       <c r="O17" s="24"/>
     </row>
     <row r="18" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="51"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="53"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="52"/>
     </row>
     <row r="19" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C19" s="51"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="53"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="52"/>
       <c r="L19" s="26" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="20" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="51"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="53"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="52"/>
       <c r="L20" s="30"/>
     </row>
     <row r="21" spans="3:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="54"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="56"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="55"/>
       <c r="L21" s="31" t="s">
         <v>39</v>
       </c>
@@ -2815,23 +2815,23 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="38" t="s">
+      <c r="K1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
       <c r="O1" s="15"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
       <c r="Z1" s="15"/>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -3073,13 +3073,13 @@
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="50"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="49"/>
       <c r="L14" s="21" t="b">
         <v>0</v>
       </c>
@@ -3098,54 +3098,54 @@
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="53"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="52"/>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="53"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="52"/>
     </row>
     <row r="17" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="51"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="53"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="52"/>
     </row>
     <row r="18" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="51"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="53"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="52"/>
     </row>
     <row r="19" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="51"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="53"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="52"/>
     </row>
     <row r="20" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="51"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="53"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="52"/>
     </row>
     <row r="21" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="54"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="56"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>